<commit_message>
Now adding B, X, and BX tabs to Paper Examples.xlsx
</commit_message>
<xml_diff>
--- a/data/BXCC.xlsx
+++ b/data/BXCC.xlsx
@@ -6,9 +6,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="B" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="X" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="BX" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="B" sheetId="7" state="visible" r:id="rId1"/>
+    <sheet name="X" sheetId="8" state="visible" r:id="rId2"/>
+    <sheet name="BX" sheetId="9" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="R__B">'B'!$A$140:$AK$144</definedName>

</xml_diff>

<commit_message>
Adding ECC to repository.
</commit_message>
<xml_diff>
--- a/data/BXCC.xlsx
+++ b/data/BXCC.xlsx
@@ -6,9 +6,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="B" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="X" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="BX" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="B" sheetId="4" state="visible" r:id="rId1"/>
+    <sheet name="X" sheetId="5" state="visible" r:id="rId2"/>
+    <sheet name="BX" sheetId="6" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="R__B">'B'!$A$140:$AK$144</definedName>

</xml_diff>